<commit_message>
Update de la planif + QA
</commit_message>
<xml_diff>
--- a/Gestion/L2 Mega_planif.xlsx
+++ b/Gestion/L2 Mega_planif.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6372" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="271">
   <si>
     <t>Objectif</t>
   </si>
@@ -866,6 +866,18 @@
   </si>
   <si>
     <t>DSK + PIC + Écran LCD + Clavier (télécommande)</t>
+  </si>
+  <si>
+    <t>2.T.2.10</t>
+  </si>
+  <si>
+    <t>Détecter la durée des notes (Rythmique)</t>
+  </si>
+  <si>
+    <t>On peut facilement détecter les rondes, blanches, noires et les croches.</t>
+  </si>
+  <si>
+    <t>2 à 3 fausses détections</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1059,15 +1071,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1078,9 +1081,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1088,6 +1088,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,36 +1424,36 @@
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="47.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1454,13 +1467,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA516"/>
+  <dimension ref="A1:AA517"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F89" sqref="F89"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,62 +1490,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
     </row>
     <row r="2" spans="1:27" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
       <c r="O2" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
@@ -3224,46 +3237,52 @@
       <c r="Z49" s="17"/>
       <c r="AA49" s="17"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C50" s="2" t="s">
+    <row r="50" spans="1:27" s="29" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="35"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="G50" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
+      <c r="P50" s="26"/>
+      <c r="Q50" s="26"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="26"/>
+      <c r="T50" s="26"/>
+      <c r="U50" s="26"/>
+      <c r="V50" s="26"/>
+      <c r="W50" s="26"/>
+      <c r="X50" s="26"/>
+      <c r="Y50" s="26"/>
+      <c r="Z50" s="26"/>
+      <c r="AA50" s="26"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C51" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
-      <c r="X50" s="2"/>
-      <c r="Y50" s="2"/>
-      <c r="Z50" s="2"/>
-      <c r="AA50" s="2"/>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A51" s="16"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3290,27 +3309,20 @@
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="D52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-      <c r="K52" s="2">
-        <v>2</v>
-      </c>
-      <c r="L52" s="2">
-        <v>4</v>
-      </c>
-      <c r="M52" s="2">
-        <f>L52*K52</f>
-        <v>8</v>
-      </c>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
@@ -3331,10 +3343,10 @@
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3344,11 +3356,11 @@
         <v>2</v>
       </c>
       <c r="L53" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" ref="M53:M54" si="3">L53*K53</f>
-        <v>2</v>
+        <f>L53*K53</f>
+        <v>8</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -3370,10 +3382,10 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3386,7 +3398,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="M54:M55" si="3">L54*K54</f>
         <v>2</v>
       </c>
       <c r="N54" s="2"/>
@@ -3405,21 +3417,29 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="F55" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
+      <c r="K55" s="2">
+        <v>2</v>
+      </c>
+      <c r="L55" s="2">
+        <v>1</v>
+      </c>
+      <c r="M55" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -3437,27 +3457,20 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="D56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="2"/>
       <c r="F56" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="2">
-        <v>2</v>
-      </c>
-      <c r="L56" s="2">
-        <v>3</v>
-      </c>
-      <c r="M56" s="2">
-        <f>L56*K56</f>
-        <v>6</v>
-      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
@@ -3477,10 +3490,10 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3490,11 +3503,11 @@
         <v>2</v>
       </c>
       <c r="L57" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" ref="M57:M58" si="4">L57*K57</f>
-        <v>20</v>
+        <f>L57*K57</f>
+        <v>6</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -3515,10 +3528,10 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3528,11 +3541,11 @@
         <v>2</v>
       </c>
       <c r="L58" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" ref="M58:M59" si="4">L58*K58</f>
+        <v>20</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -3551,20 +3564,27 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="F59" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
+      <c r="K59" s="2">
+        <v>2</v>
+      </c>
+      <c r="L59" s="2">
+        <v>2</v>
+      </c>
+      <c r="M59" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
@@ -3582,27 +3602,20 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="D60" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E60" s="2"/>
       <c r="F60" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
-      <c r="K60" s="2">
-        <v>2</v>
-      </c>
-      <c r="L60" s="2">
-        <v>3</v>
-      </c>
-      <c r="M60" s="2">
-        <f>L60*K60</f>
-        <v>6</v>
-      </c>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
@@ -3622,10 +3635,10 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3635,11 +3648,11 @@
         <v>2</v>
       </c>
       <c r="L61" s="2">
+        <v>3</v>
+      </c>
+      <c r="M61" s="2">
+        <f>L61*K61</f>
         <v>6</v>
-      </c>
-      <c r="M61" s="2">
-        <f t="shared" ref="M61:M62" si="5">L61*K61</f>
-        <v>12</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -3660,10 +3673,10 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3673,11 +3686,11 @@
         <v>2</v>
       </c>
       <c r="L62" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M62" s="2">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <f t="shared" ref="M62:M63" si="5">L62*K62</f>
+        <v>12</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -3695,22 +3708,28 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B63" s="3">
-        <v>3</v>
-      </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2" t="s">
-        <v>140</v>
+      <c r="E63" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
+      <c r="K63" s="2">
+        <v>2</v>
+      </c>
+      <c r="L63" s="2">
+        <v>4</v>
+      </c>
+      <c r="M63" s="2">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
@@ -3727,14 +3746,14 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B64" s="3"/>
-      <c r="C64" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="B64" s="3">
+        <v>3</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -3760,13 +3779,13 @@
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B65" s="3"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="C65" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3790,26 +3809,19 @@
       <c r="Z65" s="2"/>
       <c r="AA65" s="2"/>
     </row>
-    <row r="66" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="16"/>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B66" s="3"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D66" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E66" s="2"/>
       <c r="F66" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G66" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="H66" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -3829,25 +3841,25 @@
       <c r="Z66" s="2"/>
       <c r="AA66" s="2"/>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="3"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -3874,19 +3886,19 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>220</v>
+        <v>150</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -3908,20 +3920,25 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A69" s="16"/>
       <c r="B69" s="3"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
@@ -3941,24 +3958,21 @@
       <c r="Z69" s="2"/>
       <c r="AA69" s="2"/>
     </row>
-    <row r="70" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B70" s="3"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
@@ -3982,19 +3996,19 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -4017,16 +4031,22 @@
     </row>
     <row r="72" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="F72" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
@@ -4048,22 +4068,16 @@
     </row>
     <row r="73" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="D73" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E73" s="2"/>
       <c r="F73" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
@@ -4087,19 +4101,19 @@
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>187</v>
+        <v>153</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
@@ -4122,16 +4136,22 @@
     </row>
     <row r="75" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C75" s="2"/>
-      <c r="D75" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="F75" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G75" s="2"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
@@ -4153,22 +4173,16 @@
     </row>
     <row r="76" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="D76" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="G76" s="2"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
@@ -4188,20 +4202,20 @@
       <c r="Z76" s="2"/>
       <c r="AA76" s="2"/>
     </row>
-    <row r="77" spans="1:27" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G77" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="H77" s="15" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>36</v>
@@ -4225,14 +4239,23 @@
       <c r="Z77" s="2"/>
       <c r="AA77" s="2"/>
     </row>
-    <row r="78" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:27" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F78" s="2" t="s">
-        <v>148</v>
+        <v>216</v>
+      </c>
+      <c r="G78" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="H78" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -4255,21 +4278,12 @@
     </row>
     <row r="79" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2" t="s">
-        <v>173</v>
-      </c>
+      <c r="D79" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H79" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -4294,16 +4308,16 @@
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>38</v>
@@ -4331,16 +4345,20 @@
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
+        <v>203</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
@@ -4362,14 +4380,16 @@
     </row>
     <row r="82" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C82" s="2"/>
-      <c r="D82" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="F82" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G82" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
@@ -4393,16 +4413,14 @@
     </row>
     <row r="83" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="D83" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>221</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
@@ -4428,10 +4446,10 @@
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>221</v>
@@ -4461,10 +4479,10 @@
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>221</v>
@@ -4491,24 +4509,19 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="16"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2" t="s">
-        <v>253</v>
+        <v>194</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>254</v>
+        <v>160</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
@@ -4528,131 +4541,132 @@
       <c r="Z86" s="2"/>
       <c r="AA86" s="2"/>
     </row>
-    <row r="87" spans="1:27" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="16"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="29" t="s">
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
+      <c r="S87" s="2"/>
+      <c r="T87" s="2"/>
+      <c r="U87" s="2"/>
+      <c r="V87" s="2"/>
+      <c r="W87" s="2"/>
+      <c r="X87" s="2"/>
+      <c r="Y87" s="2"/>
+      <c r="Z87" s="2"/>
+      <c r="AA87" s="2"/>
+    </row>
+    <row r="88" spans="1:27" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="16"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="F87" s="29" t="s">
+      <c r="F88" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="G87" s="30" t="s">
+      <c r="G88" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="H87" s="29" t="s">
+      <c r="H88" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="I87" s="29" t="s">
+      <c r="I88" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J87" s="27"/>
-      <c r="K87" s="27"/>
-      <c r="L87" s="27"/>
-      <c r="M87" s="27"/>
-      <c r="N87" s="27"/>
-      <c r="O87" s="27"/>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="27"/>
-      <c r="R87" s="27"/>
-      <c r="S87" s="27"/>
-      <c r="T87" s="27"/>
-      <c r="U87" s="27"/>
-      <c r="V87" s="27"/>
-      <c r="W87" s="27"/>
-      <c r="X87" s="27"/>
-      <c r="Y87" s="27"/>
-      <c r="Z87" s="27"/>
-      <c r="AA87" s="27"/>
-    </row>
-    <row r="88" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="16"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="29" t="s">
+      <c r="J88" s="24"/>
+      <c r="K88" s="24"/>
+      <c r="L88" s="24"/>
+      <c r="M88" s="24"/>
+      <c r="N88" s="24"/>
+      <c r="O88" s="24"/>
+      <c r="P88" s="24"/>
+      <c r="Q88" s="24"/>
+      <c r="R88" s="24"/>
+      <c r="S88" s="24"/>
+      <c r="T88" s="24"/>
+      <c r="U88" s="24"/>
+      <c r="V88" s="24"/>
+      <c r="W88" s="24"/>
+      <c r="X88" s="24"/>
+      <c r="Y88" s="24"/>
+      <c r="Z88" s="24"/>
+      <c r="AA88" s="24"/>
+    </row>
+    <row r="89" spans="1:27" s="25" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="16"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="F88" s="29" t="s">
+      <c r="F89" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="G88" s="30" t="s">
+      <c r="G89" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="H88" s="29" t="s">
+      <c r="H89" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="I88" s="29" t="s">
+      <c r="I89" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J88" s="27"/>
-      <c r="K88" s="27"/>
-      <c r="L88" s="27"/>
-      <c r="M88" s="27"/>
-      <c r="N88" s="27"/>
-      <c r="O88" s="27"/>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="27"/>
-      <c r="R88" s="27"/>
-      <c r="S88" s="27"/>
-      <c r="T88" s="27"/>
-      <c r="U88" s="27"/>
-      <c r="V88" s="27"/>
-      <c r="W88" s="27"/>
-      <c r="X88" s="27"/>
-      <c r="Y88" s="27"/>
-      <c r="Z88" s="27"/>
-      <c r="AA88" s="27"/>
-    </row>
-    <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C89" s="2"/>
-      <c r="D89" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="2"/>
-      <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
-      <c r="P89" s="2"/>
-      <c r="Q89" s="2"/>
-      <c r="R89" s="2"/>
-      <c r="S89" s="2"/>
-      <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
-      <c r="V89" s="2"/>
-      <c r="W89" s="2"/>
-      <c r="X89" s="2"/>
-      <c r="Y89" s="2"/>
-      <c r="Z89" s="2"/>
-      <c r="AA89" s="2"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="24"/>
+      <c r="P89" s="24"/>
+      <c r="Q89" s="24"/>
+      <c r="R89" s="24"/>
+      <c r="S89" s="24"/>
+      <c r="T89" s="24"/>
+      <c r="U89" s="24"/>
+      <c r="V89" s="24"/>
+      <c r="W89" s="24"/>
+      <c r="X89" s="24"/>
+      <c r="Y89" s="24"/>
+      <c r="Z89" s="24"/>
+      <c r="AA89" s="24"/>
     </row>
     <row r="90" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2" t="s">
-        <v>213</v>
-      </c>
+      <c r="D90" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H90" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
@@ -4674,16 +4688,22 @@
     </row>
     <row r="91" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C91" s="2"/>
-      <c r="D91" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="F91" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G91" s="2"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
@@ -4705,22 +4725,16 @@
     </row>
     <row r="92" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2" t="s">
-        <v>214</v>
-      </c>
+      <c r="D92" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="H92" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G92" s="2"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
@@ -4744,13 +4758,13 @@
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>192</v>
@@ -4777,19 +4791,24 @@
       <c r="Z93" s="2"/>
       <c r="AA93" s="2"/>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B94" s="3"/>
-      <c r="C94" s="2" t="s">
-        <v>121</v>
-      </c>
+    <row r="94" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
@@ -4811,13 +4830,13 @@
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B95" s="3"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="C95" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -4844,27 +4863,20 @@
     <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B96" s="3"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="D96" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E96" s="2"/>
       <c r="F96" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
-      <c r="K96" s="2">
-        <v>2</v>
-      </c>
-      <c r="L96" s="2">
-        <v>4</v>
-      </c>
-      <c r="M96" s="2">
-        <f>L96*K96</f>
-        <v>8</v>
-      </c>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
@@ -4885,10 +4897,10 @@
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -4898,11 +4910,11 @@
         <v>2</v>
       </c>
       <c r="L97" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M97" s="2">
-        <f t="shared" ref="M97:M98" si="6">L97*K97</f>
-        <v>2</v>
+        <f>L97*K97</f>
+        <v>8</v>
       </c>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -4924,10 +4936,10 @@
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -4940,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="M98" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="M98:M99" si="6">L98*K98</f>
         <v>2</v>
       </c>
       <c r="N98" s="2"/>
@@ -4961,20 +4973,27 @@
     <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B99" s="3"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="F99" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
-      <c r="M99" s="2"/>
+      <c r="K99" s="2">
+        <v>2</v>
+      </c>
+      <c r="L99" s="2">
+        <v>1</v>
+      </c>
+      <c r="M99" s="2">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
@@ -4993,27 +5012,20 @@
     <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B100" s="3"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="D100" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E100" s="2"/>
       <c r="F100" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
-      <c r="K100" s="2">
-        <v>2</v>
-      </c>
-      <c r="L100" s="2">
-        <v>3</v>
-      </c>
-      <c r="M100" s="2">
-        <f>L100*K100</f>
-        <v>6</v>
-      </c>
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+      <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
@@ -5034,10 +5046,10 @@
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -5047,11 +5059,11 @@
         <v>2</v>
       </c>
       <c r="L101" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M101" s="2">
-        <f t="shared" ref="M101:M102" si="7">L101*K101</f>
-        <v>20</v>
+        <f>L101*K101</f>
+        <v>6</v>
       </c>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -5073,10 +5085,10 @@
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -5086,11 +5098,11 @@
         <v>2</v>
       </c>
       <c r="L102" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M102" s="2">
-        <f t="shared" si="7"/>
-        <v>4</v>
+        <f t="shared" ref="M102:M103" si="7">L102*K102</f>
+        <v>20</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -5110,20 +5122,27 @@
     <row r="103" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B103" s="3"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="F103" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
+      <c r="K103" s="2">
+        <v>2</v>
+      </c>
+      <c r="L103" s="2">
+        <v>2</v>
+      </c>
+      <c r="M103" s="2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
@@ -5142,27 +5161,20 @@
     <row r="104" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B104" s="3"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="D104" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E104" s="2"/>
       <c r="F104" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
-      <c r="K104" s="2">
-        <v>2</v>
-      </c>
-      <c r="L104" s="2">
-        <v>3</v>
-      </c>
-      <c r="M104" s="2">
-        <f>L104*K104</f>
-        <v>6</v>
-      </c>
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
@@ -5183,10 +5195,10 @@
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -5196,11 +5208,11 @@
         <v>2</v>
       </c>
       <c r="L105" s="2">
+        <v>3</v>
+      </c>
+      <c r="M105" s="2">
+        <f>L105*K105</f>
         <v>6</v>
-      </c>
-      <c r="M105" s="2">
-        <f t="shared" ref="M105:M106" si="8">L105*K105</f>
-        <v>12</v>
       </c>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -5222,10 +5234,10 @@
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -5235,11 +5247,11 @@
         <v>2</v>
       </c>
       <c r="L106" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M106" s="2">
-        <f t="shared" si="8"/>
-        <v>8</v>
+        <f t="shared" ref="M106:M107" si="8">L106*K106</f>
+        <v>12</v>
       </c>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
@@ -5256,97 +5268,109 @@
       <c r="Z106" s="2"/>
       <c r="AA106" s="2"/>
     </row>
-    <row r="107" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="16"/>
-      <c r="B107" s="32" t="s">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B107" s="3"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2">
+        <v>2</v>
+      </c>
+      <c r="L107" s="2">
+        <v>4</v>
+      </c>
+      <c r="M107" s="2">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="N107" s="2"/>
+      <c r="O107" s="2"/>
+      <c r="P107" s="2"/>
+      <c r="Q107" s="2"/>
+      <c r="R107" s="2"/>
+      <c r="S107" s="2"/>
+      <c r="T107" s="2"/>
+      <c r="U107" s="2"/>
+      <c r="V107" s="2"/>
+      <c r="W107" s="2"/>
+      <c r="X107" s="2"/>
+      <c r="Y107" s="2"/>
+      <c r="Z107" s="2"/>
+      <c r="AA107" s="2"/>
+    </row>
+    <row r="108" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="16"/>
+      <c r="B108" s="28" t="s">
         <v>264</v>
       </c>
-      <c r="C107" s="29"/>
-      <c r="D107" s="29"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29" t="s">
+      <c r="C108" s="26"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
-      <c r="L107" s="29"/>
-      <c r="M107" s="29"/>
-      <c r="N107" s="29"/>
-      <c r="O107" s="29"/>
-      <c r="P107" s="29"/>
-      <c r="Q107" s="29"/>
-      <c r="R107" s="29"/>
-      <c r="S107" s="29"/>
-      <c r="T107" s="29"/>
-      <c r="U107" s="29"/>
-      <c r="V107" s="29"/>
-      <c r="W107" s="29"/>
-      <c r="X107" s="29"/>
-      <c r="Y107" s="29"/>
-      <c r="Z107" s="29"/>
-      <c r="AA107" s="29"/>
-    </row>
-    <row r="108" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="32" t="s">
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26"/>
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+      <c r="N108" s="26"/>
+      <c r="O108" s="26"/>
+      <c r="P108" s="26"/>
+      <c r="Q108" s="26"/>
+      <c r="R108" s="26"/>
+      <c r="S108" s="26"/>
+      <c r="T108" s="26"/>
+      <c r="U108" s="26"/>
+      <c r="V108" s="26"/>
+      <c r="W108" s="26"/>
+      <c r="X108" s="26"/>
+      <c r="Y108" s="26"/>
+      <c r="Z108" s="26"/>
+      <c r="AA108" s="26"/>
+    </row>
+    <row r="109" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="28" t="s">
         <v>264</v>
       </c>
-      <c r="C108" s="34"/>
-      <c r="D108" s="34"/>
-      <c r="E108" s="34"/>
-      <c r="F108" s="29" t="s">
+      <c r="C109" s="30"/>
+      <c r="D109" s="30"/>
+      <c r="E109" s="30"/>
+      <c r="F109" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="G108" s="34"/>
-      <c r="H108" s="34"/>
-      <c r="I108" s="34"/>
-      <c r="J108" s="34"/>
-      <c r="K108" s="34"/>
-      <c r="L108" s="34"/>
-      <c r="M108" s="34"/>
-      <c r="N108" s="34"/>
-      <c r="O108" s="34"/>
-      <c r="P108" s="34"/>
-      <c r="Q108" s="34"/>
-      <c r="R108" s="34"/>
-      <c r="S108" s="34"/>
-      <c r="T108" s="34"/>
-      <c r="U108" s="34"/>
-      <c r="V108" s="34"/>
-      <c r="W108" s="34"/>
-      <c r="X108" s="34"/>
-      <c r="Y108" s="34"/>
-      <c r="Z108" s="34"/>
-      <c r="AA108" s="34"/>
-    </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="2"/>
-      <c r="P109" s="2"/>
-      <c r="Q109" s="2"/>
-      <c r="R109" s="2"/>
-      <c r="S109" s="2"/>
-      <c r="T109" s="2"/>
-      <c r="U109" s="2"/>
-      <c r="V109" s="2"/>
-      <c r="W109" s="2"/>
-      <c r="X109" s="2"/>
-      <c r="Y109" s="2"/>
-      <c r="Z109" s="2"/>
-      <c r="AA109" s="2"/>
+      <c r="G109" s="30"/>
+      <c r="H109" s="30"/>
+      <c r="I109" s="30"/>
+      <c r="J109" s="30"/>
+      <c r="K109" s="30"/>
+      <c r="L109" s="30"/>
+      <c r="M109" s="30"/>
+      <c r="N109" s="30"/>
+      <c r="O109" s="30"/>
+      <c r="P109" s="30"/>
+      <c r="Q109" s="30"/>
+      <c r="R109" s="30"/>
+      <c r="S109" s="30"/>
+      <c r="T109" s="30"/>
+      <c r="U109" s="30"/>
+      <c r="V109" s="30"/>
+      <c r="W109" s="30"/>
+      <c r="X109" s="30"/>
+      <c r="Y109" s="30"/>
+      <c r="Z109" s="30"/>
+      <c r="AA109" s="30"/>
     </row>
     <row r="110" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
@@ -16337,6 +16361,33 @@
       <c r="Z516" s="2"/>
       <c r="AA516" s="2"/>
     </row>
+    <row r="517" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C517" s="2"/>
+      <c r="D517" s="2"/>
+      <c r="E517" s="2"/>
+      <c r="F517" s="2"/>
+      <c r="G517" s="2"/>
+      <c r="H517" s="2"/>
+      <c r="I517" s="2"/>
+      <c r="J517" s="2"/>
+      <c r="K517" s="2"/>
+      <c r="L517" s="2"/>
+      <c r="M517" s="2"/>
+      <c r="N517" s="2"/>
+      <c r="O517" s="2"/>
+      <c r="P517" s="2"/>
+      <c r="Q517" s="2"/>
+      <c r="R517" s="2"/>
+      <c r="S517" s="2"/>
+      <c r="T517" s="2"/>
+      <c r="U517" s="2"/>
+      <c r="V517" s="2"/>
+      <c r="W517" s="2"/>
+      <c r="X517" s="2"/>
+      <c r="Y517" s="2"/>
+      <c r="Z517" s="2"/>
+      <c r="AA517" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B3:E3"/>
@@ -16355,7 +16406,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>